<commit_message>
2021-04-26 모집인 관리 commit
</commit_message>
<xml_diff>
--- a/src/main/document/협회TABLE.xlsx
+++ b/src/main/document/협회TABLE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5675BC0F-1874-42B9-9BF0-E80013D78DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C69E25-FEC4-4243-857F-4E459A2F70B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="테이블명세" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="226">
   <si>
     <t>테이블명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -764,10 +764,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>수정일시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>변경일시</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -838,12 +834,6 @@
     <t>PROPERTY05</t>
   </si>
   <si>
-    <t>REG_NO</t>
-  </si>
-  <si>
-    <t>UPD_NO</t>
-  </si>
-  <si>
     <t>코드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -876,14 +866,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>등록자번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수정자번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CODE_DTL_CD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -905,6 +887,22 @@
   </si>
   <si>
     <t>상세코드설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPD_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경자ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록자ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1360,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H131"/>
+  <dimension ref="A2:H134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1645,122 +1643,128 @@
       </c>
     </row>
     <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>148</v>
-      </c>
+      <c r="B18" s="4"/>
       <c r="C18" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
         <v>140</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>158</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="G18" s="4"/>
       <c r="H18" s="5" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B19" s="4"/>
       <c r="C19" s="3" t="s">
-        <v>10</v>
+        <v>186</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
-        <v>140</v>
+      <c r="E19" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="4"/>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="4"/>
-      <c r="C20" s="3" t="s">
+    <row r="22" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="4"/>
+      <c r="C22" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="5" t="s">
+      <c r="F22" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="F23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C23" t="s">
-        <v>168</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>138</v>
@@ -1769,172 +1773,170 @@
         <v>146</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>25</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C25" t="s">
+        <v>168</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C27" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H25" s="2" t="s">
+      <c r="F27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="F28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C29" s="3" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>64</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C30" s="3" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C31" s="3" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C32" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C33" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C34" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C35" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
@@ -1944,12 +1946,12 @@
         <v>146</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C36" s="3" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
@@ -1959,72 +1961,72 @@
         <v>146</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C37" s="3" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C38" s="3" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C39" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C40" s="3" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C41" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
@@ -2034,12 +2036,12 @@
         <v>146</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C42" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
@@ -2049,42 +2051,42 @@
         <v>146</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C43" s="3" t="s">
-        <v>170</v>
+        <v>73</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C44" s="3" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C45" s="3" t="s">
-        <v>27</v>
+        <v>170</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
@@ -2094,114 +2096,116 @@
         <v>146</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C46" s="3" t="s">
-        <v>61</v>
+        <v>168</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C47" s="3" t="s">
-        <v>171</v>
+        <v>27</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C48" s="3" t="s">
-        <v>172</v>
+        <v>61</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>82</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C49" s="3" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C50" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C51" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F49" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="H49" s="2" t="s">
+      <c r="F51" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C50" t="s">
-        <v>62</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C51" t="s">
-        <v>52</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C52" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C53" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>145</v>
@@ -2210,12 +2214,12 @@
         <v>146</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C54" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>145</v>
@@ -2224,172 +2228,182 @@
         <v>146</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C55" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C56" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C57" t="s">
-        <v>124</v>
+        <v>78</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
-        <v>86</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="C58" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C59" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>140</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C60" t="s">
-        <v>88</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>87</v>
+        <v>224</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G60" s="4"/>
+      <c r="H60" s="5" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C61" t="s">
-        <v>103</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>43</v>
+        <v>183</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G61" s="4"/>
+      <c r="H61" s="5" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C62" t="s">
-        <v>45</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>44</v>
+      <c r="A62" s="3"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G62" s="4"/>
+      <c r="H62" s="5" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C63" t="s">
-        <v>90</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>67</v>
+      <c r="A63" s="3"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D63" s="4"/>
+      <c r="E63" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G63" s="4"/>
+      <c r="H63" s="5" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
+        <v>86</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="C64" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C65" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C66" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>139</v>
@@ -2398,192 +2412,186 @@
         <v>146</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C67" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C68" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A69" t="s">
-        <v>95</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="C69" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C70" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C71" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C72" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C73" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C74" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="C75" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C76" t="s">
-        <v>124</v>
+        <v>33</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>140</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A77" t="s">
-        <v>98</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C77" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C78" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C79" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>132</v>
@@ -2592,60 +2600,60 @@
         <v>146</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C80" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C81" t="s">
+        <v>70</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C82" t="s">
         <v>124</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A82" t="s">
-        <v>107</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C82" t="s">
-        <v>106</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>140</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
+        <v>98</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="C83" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>140</v>
@@ -2654,85 +2662,88 @@
         <v>135</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C84" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C85" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C86" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A87" t="s">
-        <v>111</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="C87" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>140</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H87" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
+        <v>107</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C88" t="s">
+        <v>106</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H88" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C88" t="s">
-        <v>122</v>
-      </c>
-    </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A89" t="s">
-        <v>114</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="C89" t="s">
-        <v>116</v>
+        <v>33</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>140</v>
@@ -2741,48 +2752,60 @@
         <v>135</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>17</v>
+        <v>108</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C90" t="s">
-        <v>117</v>
+        <v>34</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A91" t="s">
-        <v>118</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="C91" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C92" t="s">
-        <v>121</v>
+        <v>77</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>195</v>
+        <v>112</v>
       </c>
       <c r="C93" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>140</v>
@@ -2790,196 +2813,229 @@
       <c r="F93" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G93" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="H93" s="2" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C94" t="s">
-        <v>173</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
+        <v>114</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="C95" t="s">
-        <v>198</v>
+        <v>116</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>135</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>176</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C96" t="s">
-        <v>177</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A97" t="s">
+        <v>118</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="C97" t="s">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>135</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>181</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C98" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
+        <v>123</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E98" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C99" t="s">
-        <v>183</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>197</v>
+        <v>125</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="G99" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="H99" s="2" t="s">
-        <v>184</v>
+        <v>65</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C100" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>196</v>
+        <v>137</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C101" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G101" s="1" t="s">
+      <c r="H101" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C102" t="s">
+        <v>177</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C103" t="s">
+        <v>180</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C104" t="s">
+        <v>193</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H104" s="2" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A105" t="s">
-        <v>126</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="C105" t="s">
-        <v>200</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>162</v>
+        <v>183</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>135</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>210</v>
+        <v>184</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C106" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>146</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C107" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>178</v>
+        <v>139</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H107" s="2" t="s">
-        <v>212</v>
+        <v>135</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A108" t="s">
+        <v>126</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="C108" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C109" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>178</v>
@@ -2988,12 +3044,12 @@
         <v>146</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C110" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>178</v>
@@ -3002,12 +3058,12 @@
         <v>146</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C111" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>178</v>
@@ -3016,12 +3072,12 @@
         <v>146</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C112" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>178</v>
@@ -3030,167 +3086,167 @@
         <v>146</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C113" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C114" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>184</v>
+        <v>213</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C115" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>140</v>
+        <v>178</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C116" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>196</v>
+        <v>139</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C117" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="E117" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C118" t="s">
+        <v>224</v>
+      </c>
+      <c r="E118" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F117" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H117" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A118" t="s">
-        <v>128</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C118" t="s">
-        <v>200</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="F118" s="1" t="s">
         <v>135</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C119" t="s">
-        <v>221</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>22</v>
+        <v>185</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>137</v>
+        <v>195</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C120" t="s">
+        <v>222</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H120" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E120" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H120" s="2" t="s">
-        <v>225</v>
-      </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
+        <v>128</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="C121" t="s">
-        <v>224</v>
+        <v>199</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C122" t="s">
-        <v>203</v>
+        <v>216</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C123" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>178</v>
@@ -3199,12 +3255,12 @@
         <v>146</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C124" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>178</v>
@@ -3213,12 +3269,12 @@
         <v>146</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C125" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>178</v>
@@ -3227,12 +3283,12 @@
         <v>146</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C126" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>178</v>
@@ -3241,80 +3297,122 @@
         <v>146</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C127" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C128" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>184</v>
+        <v>213</v>
       </c>
     </row>
     <row r="129" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C129" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>140</v>
+        <v>178</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="130" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C130" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>196</v>
+        <v>139</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
     </row>
     <row r="131" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C131" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="E131" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="132" spans="3:8" x14ac:dyDescent="0.4">
+      <c r="C132" t="s">
+        <v>224</v>
+      </c>
+      <c r="E132" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F131" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H131" s="2" t="s">
-        <v>220</v>
+      <c r="F132" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H132" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="133" spans="3:8" x14ac:dyDescent="0.4">
+      <c r="C133" t="s">
+        <v>185</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="134" spans="3:8" x14ac:dyDescent="0.4">
+      <c r="C134" t="s">
+        <v>222</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H134" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021-04-30 테이블 ddl 및 테이블 명세서 commit
</commit_message>
<xml_diff>
--- a/src/main/document/협회TABLE.xlsx
+++ b/src/main/document/협회TABLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D02705D-025F-43F7-ADF7-CA08869DF0D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29165403-FD94-46CB-8D70-D24EE952D4FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="276">
   <si>
     <t>테이블명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,10 +72,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전화번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>부서명</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1088,6 +1084,18 @@
   </si>
   <si>
     <t>CI값</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>휴대폰번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXTENSION_NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내선번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1588,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H155"/>
+  <dimension ref="A2:H156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1618,10 +1626,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>3</v>
@@ -1632,42 +1640,42 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
@@ -1675,10 +1683,10 @@
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>10</v>
@@ -1686,30 +1694,30 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
@@ -1717,184 +1725,183 @@
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5" t="s">
-        <v>13</v>
+      <c r="E10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="5" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="5" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C13" s="3" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>270</v>
+        <v>82</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>76</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C14" s="3" t="s">
-        <v>209</v>
+        <v>93</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>80</v>
+        <v>269</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="4"/>
       <c r="H14" s="5" t="s">
-        <v>210</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B15" s="4"/>
       <c r="C15" s="3" t="s">
-        <v>70</v>
+        <v>208</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="G15" s="4"/>
       <c r="H15" s="5" t="s">
-        <v>71</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B16" s="4"/>
       <c r="C16" s="3" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B17" s="4"/>
       <c r="C17" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="H17" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B18" s="4"/>
       <c r="C18" s="3" t="s">
-        <v>153</v>
+        <v>90</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="H18" s="5" t="s">
-        <v>154</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
@@ -1903,197 +1910,194 @@
         <v>152</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="12" t="s">
-        <v>118</v>
+      <c r="E19" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="4"/>
+      <c r="C20" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="D21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="4"/>
-      <c r="C21" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="4"/>
       <c r="H21" s="5" t="s">
-        <v>149</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B22" s="4"/>
       <c r="C22" s="3" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="4"/>
+      <c r="C23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C24" t="s">
-        <v>159</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C25" t="s">
-        <v>160</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>194</v>
+        <v>158</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>77</v>
+        <v>193</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C27" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>72</v>
+        <v>160</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A28" s="7" t="s">
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A29" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
       <c r="C29" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G29" s="8"/>
       <c r="H29" s="9" t="s">
@@ -2101,645 +2105,647 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" t="s">
         <v>164</v>
       </c>
-      <c r="C30" t="s">
-        <v>165</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C31" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>75</v>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>148</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C32" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C33" s="3" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>270</v>
+        <v>79</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>255</v>
+        <v>74</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>254</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C34" s="3" t="s">
-        <v>52</v>
+        <v>165</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>247</v>
+        <v>83</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C35" s="3" t="s">
-        <v>167</v>
+        <v>51</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>78</v>
+        <v>269</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C36" s="3" t="s">
-        <v>242</v>
+        <v>166</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
-        <v>270</v>
+        <v>77</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C37" s="3" t="s">
-        <v>169</v>
+        <v>241</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G37" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>263</v>
+      </c>
       <c r="H37" s="5" t="s">
-        <v>22</v>
+        <v>251</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C38" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>72</v>
+        <v>269</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C39" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.4">
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" s="4"/>
+      <c r="H40" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.4">
+      <c r="C41" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G41" s="8"/>
+      <c r="H41" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G40" s="8"/>
-      <c r="H40" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.4">
-      <c r="C41" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G41" s="4"/>
-      <c r="H41" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C42" s="3" t="s">
-        <v>231</v>
+        <v>171</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5" t="s">
-        <v>232</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C43" s="3" t="s">
-        <v>173</v>
+        <v>230</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="5" t="s">
-        <v>29</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C44" s="3" t="s">
-        <v>40</v>
+        <v>172</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>271</v>
+        <v>71</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>258</v>
+        <v>83</v>
+      </c>
+      <c r="G44" s="4"/>
+      <c r="H44" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C45" s="3" t="s">
-        <v>259</v>
+        <v>39</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
-        <v>81</v>
+        <v>270</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C46" s="3" t="s">
-        <v>174</v>
+        <v>258</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
         <v>80</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>39</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C47" s="3" t="s">
-        <v>236</v>
+        <v>173</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C48" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C49" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C50" s="3" t="s">
-        <v>175</v>
+        <v>237</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C51" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C52" s="3" t="s">
-        <v>245</v>
+        <v>175</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4" t="s">
         <v>77</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G52" s="4"/>
-      <c r="H52" s="5" t="s">
-        <v>244</v>
+        <v>83</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C53" s="3" t="s">
-        <v>160</v>
+        <v>244</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>194</v>
+        <v>76</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>15</v>
+        <v>83</v>
+      </c>
+      <c r="G53" s="4"/>
+      <c r="H53" s="5" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C54" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4" t="s">
-        <v>77</v>
+        <v>193</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C55" s="3" t="s">
-        <v>37</v>
+        <v>160</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C56" s="3" t="s">
-        <v>239</v>
+        <v>36</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C57" s="3" t="s">
-        <v>49</v>
+        <v>238</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.4">
-      <c r="C58" t="s">
-        <v>177</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>84</v>
+      <c r="C58" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C59" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>83</v>
+        <v>269</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.4">
-      <c r="C60" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F60" s="8" t="s">
+      <c r="C60" t="s">
+        <v>177</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.4">
+      <c r="C61" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G61" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G60" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.4">
-      <c r="C61" t="s">
-        <v>179</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>33</v>
+      <c r="H61" s="9" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C62" t="s">
-        <v>241</v>
+        <v>178</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C63" t="s">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C64" t="s">
-        <v>46</v>
+        <v>179</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C65" t="s">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C66" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>184</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C67" t="s">
+        <v>181</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H67" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C68" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>210</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C69" t="s">
-        <v>211</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G69" s="4"/>
-      <c r="H69" s="5" t="s">
-        <v>109</v>
+        <v>207</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A70" s="3"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4" t="s">
-        <v>80</v>
+      <c r="C70" t="s">
+        <v>210</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G70" s="4"/>
       <c r="H70" s="5" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.4">
@@ -2749,1319 +2755,1337 @@
         <v>152</v>
       </c>
       <c r="D71" s="4"/>
-      <c r="E71" s="12" t="s">
-        <v>118</v>
+      <c r="E71" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G71" s="4"/>
       <c r="H71" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A72" t="s">
-        <v>51</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>196</v>
-      </c>
+      <c r="A72" s="3"/>
+      <c r="B72" s="4"/>
       <c r="C72" s="3" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="D72" s="4"/>
-      <c r="E72" s="4" t="s">
-        <v>80</v>
+      <c r="E72" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>234</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="G72" s="4"/>
       <c r="H72" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C73" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G73" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="H73" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C74" s="3" t="s">
-        <v>52</v>
+        <v>191</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="5" t="s">
-        <v>247</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C75" s="3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G75" s="4"/>
       <c r="H75" s="5" t="s">
-        <v>90</v>
+        <v>246</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C76" s="3" t="s">
-        <v>246</v>
+        <v>9</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G76" s="4"/>
       <c r="H76" s="5" t="s">
-        <v>269</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C77" s="3" t="s">
-        <v>172</v>
+        <v>245</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G77" s="4"/>
       <c r="H77" s="5" t="s">
-        <v>25</v>
+        <v>268</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C78" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F78" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="G78" s="14"/>
-      <c r="H78" s="15" t="s">
-        <v>249</v>
+      <c r="C78" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G78" s="4"/>
+      <c r="H78" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C79" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G79" s="4"/>
-      <c r="H79" s="5" t="s">
-        <v>39</v>
+      <c r="C79" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F79" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G79" s="14"/>
+      <c r="H79" s="15" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C80" s="3" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G80" s="4"/>
       <c r="H80" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C81" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G81" s="4"/>
       <c r="H81" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C82" s="3" t="s">
-        <v>53</v>
+        <v>236</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G82" s="4"/>
       <c r="H82" s="5" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C83" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G83" s="4"/>
       <c r="H83" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C84" s="3" t="s">
-        <v>208</v>
+        <v>54</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G84" s="4"/>
       <c r="H84" s="5" t="s">
-        <v>243</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A85" t="s">
-        <v>57</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="C85" s="3" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G85" s="4" t="s">
-        <v>234</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="G85" s="4"/>
       <c r="H85" s="5" t="s">
-        <v>189</v>
+        <v>242</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
+        <v>56</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="C86" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G86" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="H86" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C87" s="3" t="s">
-        <v>52</v>
+        <v>191</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G87" s="4"/>
       <c r="H87" s="5" t="s">
-        <v>247</v>
+        <v>192</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C88" s="3" t="s">
-        <v>250</v>
+        <v>51</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="5" t="s">
-        <v>24</v>
+        <v>246</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C89" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F89" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="G89" s="14"/>
-      <c r="H89" s="15" t="s">
+      <c r="C89" s="3" t="s">
         <v>249</v>
       </c>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G89" s="4"/>
+      <c r="H89" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C90" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D90" s="4"/>
-      <c r="E90" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F90" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G90" s="4"/>
-      <c r="H90" s="5" t="s">
-        <v>25</v>
+      <c r="C90" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F90" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G90" s="14"/>
+      <c r="H90" s="15" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C91" s="3" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G91" s="4"/>
       <c r="H91" s="5" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C92" s="3" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C93" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C94" s="3" t="s">
-        <v>208</v>
+        <v>236</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="5" t="s">
-        <v>243</v>
+        <v>41</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A95" t="s">
-        <v>58</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="C95" s="3" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G95" s="4" t="s">
-        <v>234</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="G95" s="4"/>
       <c r="H95" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
+        <v>57</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C96" s="3" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G96" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="H96" s="5" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C97" s="3" t="s">
-        <v>251</v>
+        <v>191</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="5" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C98" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>25</v>
+        <v>250</v>
+      </c>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G98" s="4"/>
+      <c r="H98" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C99" t="s">
-        <v>208</v>
+      <c r="C99" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>243</v>
+        <v>24</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A100" t="s">
-        <v>59</v>
-      </c>
-      <c r="B100" s="1" t="s">
+      <c r="C100" t="s">
+        <v>207</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A101" t="s">
+        <v>58</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C101" t="s">
         <v>201</v>
       </c>
-      <c r="C100" t="s">
+      <c r="E101" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H101" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C101" t="s">
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C102" t="s">
+        <v>191</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H102" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E101" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H101" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C102" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D102" s="4"/>
-      <c r="E102" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F102" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H102" s="2" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C103" t="s">
-        <v>240</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>84</v>
+      <c r="C103" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C104" t="s">
-        <v>45</v>
+        <v>239</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A105" t="s">
-        <v>61</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="C105" t="s">
-        <v>229</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G105" s="1" t="s">
-        <v>234</v>
+        <v>83</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>230</v>
+        <v>35</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A106" t="s">
+        <v>60</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="C106" t="s">
+        <v>228</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C107" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A108" t="s">
+        <v>61</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C108" t="s">
+        <v>226</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C109" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A110" t="s">
+        <v>63</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C110" t="s">
+        <v>224</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C111" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A112" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A107" t="s">
-        <v>62</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C107" t="s">
-        <v>227</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H107" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C108" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A109" t="s">
-        <v>64</v>
-      </c>
-      <c r="B109" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C109" t="s">
-        <v>225</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H109" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C110" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A111" t="s">
-        <v>67</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
+        <v>208</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H112" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="H111" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C112" t="s">
-        <v>256</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="H112" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C113" t="s">
-        <v>116</v>
+        <v>255</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>115</v>
+        <v>260</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>114</v>
+        <v>256</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C114" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C115" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C116" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C117" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C118" t="s">
-        <v>211</v>
-      </c>
-      <c r="E118" s="6" t="s">
-        <v>118</v>
+        <v>106</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C119" t="s">
-        <v>152</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>118</v>
+        <v>210</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C120" t="s">
+        <v>151</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C121" t="s">
+        <v>111</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G121" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E120" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G120" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H120" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A121" t="s">
-        <v>68</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C121" t="s">
-        <v>120</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="H121" s="2" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A122" t="s">
+        <v>67</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="C122" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C123" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C124" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C125" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C126" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C127" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C128" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C129" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C130" t="s">
-        <v>211</v>
+        <v>110</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C131" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C132" t="s">
-        <v>152</v>
+        <v>185</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>110</v>
+        <v>186</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C133" t="s">
+        <v>151</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C134" t="s">
+        <v>152</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H134" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E133" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H133" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A134" t="s">
-        <v>69</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C134" t="s">
-        <v>120</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F134" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H134" s="2" t="s">
-        <v>128</v>
-      </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A135" t="s">
+        <v>68</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="C135" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C136" t="s">
-        <v>139</v>
+        <v>136</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C137" t="s">
+        <v>138</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H137" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H137" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C138" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C139" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C140" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C141" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C142" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C143" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C144" t="s">
-        <v>211</v>
+        <v>110</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C145" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H145" s="2" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C146" t="s">
-        <v>152</v>
+        <v>185</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C147" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H147" s="2" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A148" t="s">
-        <v>214</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>215</v>
+      <c r="C148" t="s">
+        <v>152</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
+        <v>215</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A151" t="s">
+        <v>217</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C150" t="s">
-        <v>171</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F150" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H150" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C151" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C152" t="s">
-        <v>166</v>
+        <v>171</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>221</v>
+        <v>27</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C153" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C154" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C155" t="s">
-        <v>220</v>
+        <v>173</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H155" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C156" t="s">
+        <v>219</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H156" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -4099,16 +4123,16 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>130</v>
-      </c>
       <c r="E2" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>

</xml_diff>

<commit_message>
2021-04-30 코드 샘플 추가 및 table명세서 수정 commit
</commit_message>
<xml_diff>
--- a/src/main/document/협회TABLE.xlsx
+++ b/src/main/document/협회TABLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235E60B8-F814-415A-9998-C4DC6F1D3802}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1A8C54-10E5-4D31-B466-FEE3625D1643}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="284">
   <si>
     <t>테이블명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1117,6 +1117,15 @@
   <si>
     <t>TERMS_DATE</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tb_lc_mas01_imwon_seq</t>
+  </si>
+  <si>
+    <t>tb_lc_mas01_expert_seq</t>
+  </si>
+  <si>
+    <t>tb_lc_mas01_it_seq</t>
   </si>
 </sst>
 </file>
@@ -1618,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H158"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J100" sqref="J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2859,7 +2868,7 @@
         <v>74</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>233</v>
+        <v>281</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>189</v>
@@ -2892,7 +2901,9 @@
       <c r="F77" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G77" s="4"/>
+      <c r="G77" s="4" t="s">
+        <v>261</v>
+      </c>
       <c r="H77" s="5" t="s">
         <v>246</v>
       </c>
@@ -3075,7 +3086,7 @@
         <v>74</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>233</v>
+        <v>282</v>
       </c>
       <c r="H88" s="5" t="s">
         <v>188</v>
@@ -3172,7 +3183,9 @@
       <c r="F94" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G94" s="4"/>
+      <c r="G94" s="4" t="s">
+        <v>261</v>
+      </c>
       <c r="H94" s="5" t="s">
         <v>38</v>
       </c>
@@ -3243,7 +3256,7 @@
         <v>74</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>233</v>
+        <v>283</v>
       </c>
       <c r="H98" s="5" t="s">
         <v>198</v>

</xml_diff>

<commit_message>
2021-05-21 모집인 승인처리 commit
</commit_message>
<xml_diff>
--- a/src/main/document/협회TABLE.xlsx
+++ b/src/main/document/협회TABLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E092E3E-4609-4DDE-AABA-DABF65B440A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF9236A-5AA8-4A7F-96A7-DC8254672EC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="330">
   <si>
     <t>테이블명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1273,6 +1273,30 @@
   </si>
   <si>
     <t>위반이력코드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>첨부서류체크정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB_LC_FILE_CHECK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHECK_CD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>첨부서류체크코드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CORP_USER_YN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>법인사용인여부</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1331,7 +1355,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1375,6 +1399,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1764,10 +1791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K195"/>
+  <dimension ref="A2:K198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D183" sqref="D183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2523,62 +2550,62 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="C44" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>228</v>
+      <c r="C44" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C45" s="3" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
-        <v>70</v>
+        <v>249</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C46" s="3" t="s">
-        <v>223</v>
+        <v>152</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
-        <v>249</v>
+        <v>70</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>20</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C47" s="3" t="s">
-        <v>153</v>
+        <v>223</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4" t="s">
@@ -2588,29 +2615,28 @@
         <v>76</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="H47" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
+        <v>243</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C48" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4" t="s">
-        <v>64</v>
+        <v>249</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G48" s="4"/>
-      <c r="H48" s="5" t="s">
-        <v>21</v>
+      <c r="G48" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>298</v>
       </c>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
@@ -2618,7 +2644,7 @@
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C49" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
@@ -2629,7 +2655,7 @@
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
@@ -2637,18 +2663,18 @@
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C50" s="3" t="s">
-        <v>251</v>
+        <v>155</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="5" t="s">
-        <v>252</v>
+        <v>25</v>
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
@@ -2656,18 +2682,18 @@
     </row>
     <row r="51" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C51" s="3" t="s">
-        <v>156</v>
+        <v>251</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="5" t="s">
-        <v>26</v>
+        <v>252</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
@@ -2675,7 +2701,7 @@
     </row>
     <row r="52" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C52" s="3" t="s">
-        <v>213</v>
+        <v>156</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4" t="s">
@@ -2686,7 +2712,7 @@
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="5" t="s">
-        <v>214</v>
+        <v>26</v>
       </c>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
@@ -2694,7 +2720,7 @@
     </row>
     <row r="53" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C53" s="3" t="s">
-        <v>157</v>
+        <v>213</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
@@ -2705,7 +2731,7 @@
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="5" t="s">
-        <v>27</v>
+        <v>214</v>
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
@@ -2713,20 +2739,18 @@
     </row>
     <row r="54" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C54" s="3" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4" t="s">
-        <v>250</v>
+        <v>64</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G54" s="4" t="s">
-        <v>256</v>
-      </c>
+      <c r="G54" s="4"/>
       <c r="H54" s="5" t="s">
-        <v>237</v>
+        <v>27</v>
       </c>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
@@ -2734,18 +2758,20 @@
     </row>
     <row r="55" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C55" s="3" t="s">
-        <v>238</v>
+        <v>38</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
-        <v>73</v>
+        <v>250</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G55" s="4"/>
+      <c r="G55" s="4" t="s">
+        <v>256</v>
+      </c>
       <c r="H55" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
@@ -2753,37 +2779,41 @@
     </row>
     <row r="56" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C56" s="3" t="s">
-        <v>158</v>
+        <v>238</v>
       </c>
       <c r="D56" s="4"/>
-      <c r="E56" s="8" t="s">
-        <v>64</v>
+      <c r="E56" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="G56" s="4"/>
+      <c r="H56" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
     </row>
     <row r="57" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C57" s="3" t="s">
-        <v>218</v>
+        <v>158</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>76</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C58" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
@@ -2793,12 +2823,12 @@
         <v>76</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C59" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
@@ -2808,12 +2838,12 @@
         <v>76</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C60" s="3" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
@@ -2823,192 +2853,190 @@
         <v>76</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C61" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F61" s="4" t="s">
         <v>76</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C62" s="3" t="s">
-        <v>226</v>
+        <v>160</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G62" s="4"/>
-      <c r="H62" s="5" t="s">
-        <v>225</v>
+      <c r="H62" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C63" s="3" t="s">
-        <v>145</v>
+        <v>226</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>178</v>
+        <v>69</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H63" s="2" t="s">
-        <v>14</v>
+      <c r="G63" s="4"/>
+      <c r="H63" s="5" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C64" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>69</v>
+        <v>178</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>76</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C65" s="3" t="s">
-        <v>35</v>
+        <v>146</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F65" s="4" t="s">
         <v>76</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C66" s="3" t="s">
-        <v>221</v>
+        <v>35</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G66" s="4"/>
-      <c r="H66" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I66" s="3"/>
+      <c r="H66" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="67" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C67" s="3" t="s">
-        <v>46</v>
+        <v>221</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I67" s="3"/>
     </row>
     <row r="68" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C68" s="3" t="s">
-        <v>161</v>
+        <v>46</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
-        <v>249</v>
+        <v>72</v>
       </c>
       <c r="F68" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G68" s="4"/>
       <c r="H68" s="5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="I68" s="3"/>
     </row>
     <row r="69" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C69" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>75</v>
+        <v>249</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G69" s="4"/>
       <c r="H69" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I69" s="3"/>
     </row>
     <row r="70" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C70" s="3" t="s">
-        <v>245</v>
+        <v>162</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>68</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="G70" s="4"/>
       <c r="H70" s="5" t="s">
-        <v>244</v>
+        <v>30</v>
       </c>
       <c r="I70" s="3"/>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C71" s="3" t="s">
-        <v>163</v>
+        <v>245</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G71" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="H71" s="5" t="s">
-        <v>31</v>
+        <v>244</v>
       </c>
       <c r="I71" s="3"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C72" s="3" t="s">
-        <v>222</v>
+        <v>163</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4" t="s">
@@ -3019,13 +3047,13 @@
       </c>
       <c r="G72" s="4"/>
       <c r="H72" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I72" s="3"/>
     </row>
     <row r="73" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C73" s="3" t="s">
-        <v>164</v>
+        <v>222</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
@@ -3036,81 +3064,81 @@
       </c>
       <c r="G73" s="4"/>
       <c r="H73" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I73" s="3"/>
     </row>
     <row r="74" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C74" s="3" t="s">
-        <v>43</v>
+        <v>164</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F74" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I74" s="3"/>
     </row>
     <row r="75" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C75" s="3" t="s">
-        <v>165</v>
+        <v>43</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>302</v>
+        <v>73</v>
       </c>
       <c r="F75" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G75" s="4"/>
       <c r="H75" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I75" s="3"/>
+    </row>
+    <row r="76" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C76" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G76" s="4"/>
+      <c r="H76" s="5" t="s">
         <v>299</v>
-      </c>
-      <c r="I75" s="3"/>
-    </row>
-    <row r="76" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="C76" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F76" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G76" s="8"/>
-      <c r="H76" s="9" t="s">
-        <v>300</v>
       </c>
       <c r="I76" s="3"/>
     </row>
     <row r="77" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C77" s="3" t="s">
-        <v>166</v>
+        <v>301</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F77" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G77" s="4"/>
       <c r="H77" s="5" t="s">
-        <v>168</v>
+        <v>300</v>
       </c>
       <c r="I77" s="3"/>
     </row>
     <row r="78" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C78" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4" t="s">
@@ -3121,60 +3149,58 @@
       </c>
       <c r="G78" s="4"/>
       <c r="H78" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I78" s="3"/>
     </row>
     <row r="79" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C79" s="3" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F79" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G79" s="4"/>
       <c r="H79" s="5" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="I79" s="3"/>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C80" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D80" s="4"/>
-      <c r="E80" s="12" t="s">
-        <v>105</v>
+      <c r="E80" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="F80" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G80" s="4"/>
       <c r="H80" s="5" t="s">
-        <v>96</v>
+        <v>193</v>
       </c>
       <c r="I80" s="3"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A81" s="3"/>
-      <c r="B81" s="4"/>
       <c r="C81" s="3" t="s">
-        <v>140</v>
+        <v>194</v>
       </c>
       <c r="D81" s="4"/>
-      <c r="E81" s="4" t="s">
-        <v>72</v>
+      <c r="E81" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F81" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G81" s="4"/>
       <c r="H81" s="5" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="I81" s="3"/>
     </row>
@@ -3182,47 +3208,48 @@
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D82" s="4"/>
-      <c r="E82" s="12" t="s">
-        <v>105</v>
+      <c r="E82" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="F82" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G82" s="4"/>
       <c r="H82" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I82" s="3"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A83" s="3"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D83" s="4"/>
+      <c r="E83" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G83" s="4"/>
+      <c r="H83" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A83" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
         <v>48</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="D83" s="4"/>
-      <c r="E83" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G83" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="H83" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C84" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
@@ -3231,48 +3258,50 @@
       <c r="F84" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G84" s="4"/>
+      <c r="G84" s="4" t="s">
+        <v>261</v>
+      </c>
       <c r="H84" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C85" s="3" t="s">
-        <v>49</v>
+        <v>176</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G85" s="4" t="s">
-        <v>241</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G85" s="4"/>
       <c r="H85" s="5" t="s">
-        <v>228</v>
+        <v>177</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C86" s="3" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G86" s="4"/>
+      <c r="G86" s="4" t="s">
+        <v>241</v>
+      </c>
       <c r="H86" s="5" t="s">
-        <v>79</v>
+        <v>228</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C87" s="3" t="s">
-        <v>227</v>
+        <v>9</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
@@ -3283,12 +3312,12 @@
       </c>
       <c r="G87" s="4"/>
       <c r="H87" s="5" t="s">
-        <v>248</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C88" s="3" t="s">
-        <v>156</v>
+        <v>227</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
@@ -3299,15 +3328,15 @@
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="5" t="s">
-        <v>23</v>
+        <v>248</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C89" s="3" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="D89" s="4"/>
-      <c r="E89" s="8" t="s">
+      <c r="E89" s="4" t="s">
         <v>64</v>
       </c>
       <c r="F89" s="4" t="s">
@@ -3315,28 +3344,28 @@
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C90" s="3" t="s">
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F90" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C91" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
@@ -3347,88 +3376,86 @@
       </c>
       <c r="G91" s="4"/>
       <c r="H91" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C92" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G92" s="4"/>
+      <c r="H92" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C92" s="7" t="s">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C93" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8" t="s">
+      <c r="D93" s="4"/>
+      <c r="E93" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F92" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G92" s="8" t="s">
+      <c r="F93" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G93" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="H92" s="9" t="s">
+      <c r="H93" s="5" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C93" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F93" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G93" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="H93" s="9" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C94" s="3" t="s">
-        <v>191</v>
+        <v>286</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F94" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G94" s="4"/>
+      <c r="G94" s="4" t="s">
+        <v>289</v>
+      </c>
       <c r="H94" s="5" t="s">
-        <v>224</v>
+        <v>287</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A95" t="s">
-        <v>50</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="C95" s="3" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G95" s="4" t="s">
-        <v>262</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="G95" s="4"/>
       <c r="H95" s="5" t="s">
-        <v>173</v>
+        <v>224</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
+        <v>50</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="C96" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
@@ -3437,46 +3464,48 @@
       <c r="F96" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G96" s="4"/>
+      <c r="G96" s="4" t="s">
+        <v>262</v>
+      </c>
       <c r="H96" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C97" s="3" t="s">
-        <v>49</v>
+        <v>176</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="5" t="s">
-        <v>228</v>
+        <v>177</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C98" s="3" t="s">
-        <v>230</v>
+        <v>49</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F98" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="5" t="s">
-        <v>22</v>
+        <v>228</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C99" s="3" t="s">
-        <v>156</v>
+        <v>230</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4" t="s">
@@ -3487,46 +3516,46 @@
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C100" s="3" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="D100" s="4"/>
-      <c r="E100" s="8" t="s">
+      <c r="E100" s="4" t="s">
         <v>64</v>
       </c>
       <c r="F100" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G100" s="4" t="s">
-        <v>241</v>
-      </c>
+      <c r="G100" s="4"/>
       <c r="H100" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C101" s="3" t="s">
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F101" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G101" s="4"/>
+      <c r="G101" s="4" t="s">
+        <v>241</v>
+      </c>
       <c r="H101" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C102" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4" t="s">
@@ -3537,52 +3566,50 @@
       </c>
       <c r="G102" s="4"/>
       <c r="H102" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C103" s="3" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F103" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="5" t="s">
-        <v>224</v>
+        <v>40</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A104" t="s">
-        <v>51</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="C104" s="3" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G104" s="4" t="s">
-        <v>263</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="G104" s="4"/>
       <c r="H104" s="5" t="s">
-        <v>183</v>
+        <v>224</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A105" t="s">
+        <v>51</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="C105" s="3" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
@@ -3591,297 +3618,304 @@
       <c r="F105" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G105" s="4"/>
+      <c r="G105" s="4" t="s">
+        <v>263</v>
+      </c>
       <c r="H105" s="5" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C106" s="3" t="s">
-        <v>231</v>
+        <v>176</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G106" s="4"/>
       <c r="H106" s="5" t="s">
-        <v>22</v>
+        <v>177</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C107" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G107" s="4"/>
+      <c r="H107" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C108" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E107" s="1" t="s">
+      <c r="D108" s="4"/>
+      <c r="E108" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F107" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H107" s="2" t="s">
+      <c r="F108" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G108" s="4"/>
+      <c r="H108" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C108" t="s">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C109" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="D109" s="4"/>
+      <c r="E109" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F108" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H108" s="2" t="s">
+      <c r="F109" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G109" s="4"/>
+      <c r="H109" s="5" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A109" t="s">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A110" t="s">
         <v>52</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C109" s="7" t="s">
+      <c r="C110" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="D109" s="8"/>
-      <c r="E109" s="8" t="s">
+      <c r="D110" s="4"/>
+      <c r="E110" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F109" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G109" s="8" t="s">
+      <c r="F110" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G110" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="H109" s="9" t="s">
+      <c r="H110" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C110" s="7" t="s">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C111" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8" t="s">
+      <c r="D111" s="4"/>
+      <c r="E111" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F110" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G110" s="8"/>
-      <c r="H110" s="9" t="s">
+      <c r="F111" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G111" s="4"/>
+      <c r="H111" s="5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C111" s="7" t="s">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C112" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8" t="s">
+      <c r="D112" s="4"/>
+      <c r="E112" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="F111" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G111" s="8"/>
-      <c r="H111" s="9" t="s">
+      <c r="F112" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G112" s="4"/>
+      <c r="H112" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C112" s="7" t="s">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C113" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8" t="s">
+      <c r="D113" s="4"/>
+      <c r="E113" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="F112" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G112" s="8"/>
-      <c r="H112" s="9" t="s">
+      <c r="F113" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G113" s="4"/>
+      <c r="H113" s="5" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C113" s="7" t="s">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C114" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8" t="s">
+      <c r="D114" s="4"/>
+      <c r="E114" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F113" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G113" s="8"/>
-      <c r="H113" s="9" t="s">
+      <c r="F114" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G114" s="4"/>
+      <c r="H114" s="5" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C114" s="7" t="s">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C115" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D114" s="8"/>
-      <c r="E114" s="8" t="s">
+      <c r="D115" s="4"/>
+      <c r="E115" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F114" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G114" s="8"/>
-      <c r="H114" s="9" t="s">
+      <c r="F115" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G115" s="4"/>
+      <c r="H115" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C115" s="7" t="s">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C116" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8" t="s">
+      <c r="D116" s="4"/>
+      <c r="E116" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F115" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G115" s="8"/>
-      <c r="H115" s="9" t="s">
+      <c r="F116" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G116" s="4"/>
+      <c r="H116" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A116" t="s">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A117" t="s">
         <v>53</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C117" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D117" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E116" s="1" t="s">
+      <c r="E117" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F116" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G116" s="1" t="s">
+      <c r="F117" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G117" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="H116" s="2" t="s">
+      <c r="H117" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C117" t="s">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C118" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A118" t="s">
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="5"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A119" t="s">
         <v>54</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B119" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C119" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D119" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="E119" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F118" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G118" s="1" t="s">
+      <c r="F119" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G119" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="H118" s="2" t="s">
+      <c r="H119" s="5" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C119" t="s">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C120" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A120" t="s">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
         <v>56</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C121" t="s">
         <v>208</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E120" s="1" t="s">
+      <c r="E121" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F120" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G120" s="1" t="s">
+      <c r="F121" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G121" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H120" s="2" t="s">
+      <c r="H121" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C121" t="s">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C122" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A122" t="s">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A123" t="s">
         <v>59</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B123" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C123" t="s">
         <v>192</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H122" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C123" t="s">
-        <v>235</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>13</v>
@@ -3893,170 +3927,176 @@
         <v>67</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>236</v>
+        <v>193</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C124" t="s">
-        <v>103</v>
+        <v>235</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>102</v>
+        <v>240</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>101</v>
+        <v>236</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C125" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>69</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C126" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C127" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C128" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C129" t="s">
-        <v>194</v>
-      </c>
-      <c r="E129" s="6" t="s">
-        <v>105</v>
+        <v>94</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C130" t="s">
-        <v>139</v>
-      </c>
-      <c r="E130" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E130" s="6" t="s">
         <v>105</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C131" t="s">
+        <v>139</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C132" t="s">
         <v>99</v>
       </c>
-      <c r="E131" s="1" t="s">
+      <c r="E132" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F131" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G131" s="1" t="s">
+      <c r="F132" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G132" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H131" s="2" t="s">
+      <c r="H132" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A132" t="s">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A133" t="s">
         <v>60</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B133" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C133" t="s">
         <v>107</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="D133" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E132" s="1" t="s">
+      <c r="E133" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F132" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H132" s="2" t="s">
+      <c r="F133" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H133" s="2" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C133" t="s">
-        <v>108</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H133" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C134" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>92</v>
@@ -4065,12 +4105,12 @@
         <v>76</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C135" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>92</v>
@@ -4079,12 +4119,12 @@
         <v>76</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C136" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>92</v>
@@ -4093,12 +4133,12 @@
         <v>76</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C137" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>92</v>
@@ -4107,12 +4147,12 @@
         <v>76</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C138" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>92</v>
@@ -4121,12 +4161,12 @@
         <v>76</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C139" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>92</v>
@@ -4135,139 +4175,139 @@
         <v>76</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C140" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C141" t="s">
-        <v>194</v>
+        <v>98</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="G141" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="H141" s="2" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C142" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C143" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>97</v>
+        <v>171</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C144" t="s">
+        <v>139</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H144" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C145" t="s">
         <v>140</v>
       </c>
-      <c r="E144" s="1" t="s">
+      <c r="E145" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F144" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H144" s="2" t="s">
+      <c r="F145" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H145" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A145" t="s">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A146" t="s">
         <v>61</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B146" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C146" t="s">
         <v>107</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F145" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H145" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C146" t="s">
-        <v>124</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C147" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C148" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>92</v>
@@ -4276,12 +4316,12 @@
         <v>76</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C149" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>92</v>
@@ -4290,12 +4330,12 @@
         <v>76</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C150" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>92</v>
@@ -4304,12 +4344,12 @@
         <v>76</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C151" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>92</v>
@@ -4318,12 +4358,12 @@
         <v>76</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C152" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>92</v>
@@ -4332,12 +4372,12 @@
         <v>76</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C153" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>92</v>
@@ -4346,576 +4386,660 @@
         <v>76</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C154" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G154" s="1" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C155" t="s">
-        <v>194</v>
+        <v>98</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="G155" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="H155" s="2" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C156" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C157" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C158" t="s">
+        <v>139</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H158" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C159" t="s">
         <v>140</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H158" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A159" t="s">
-        <v>270</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="C159" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>72</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G159" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H159" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A160" t="s">
+        <v>270</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C160" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G160" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="H159" s="14" t="s">
+      <c r="H160" s="14" t="s">
         <v>272</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C160" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F160" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H160" s="14" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C161" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>279</v>
+        <v>65</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H161" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C162" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>72</v>
+        <v>279</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G162" s="1">
-        <v>0</v>
-      </c>
       <c r="H162" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C163" s="14" t="s">
-        <v>191</v>
+        <v>278</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>72</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="G163" s="1">
+        <v>0</v>
       </c>
       <c r="H163" s="14" t="s">
-        <v>224</v>
+        <v>275</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C164" s="14" t="s">
-        <v>280</v>
+        <v>191</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G164" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="H164" s="14" t="s">
-        <v>281</v>
+        <v>224</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C165" s="14" t="s">
-        <v>194</v>
+        <v>280</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="G165" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="H165" s="14" t="s">
-        <v>96</v>
+        <v>281</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C166" s="14" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H166" s="14" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C167" s="14" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H167" s="14" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C168" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H168" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C169" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="E168" s="1" t="s">
+      <c r="E169" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F168" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H168" s="14" t="s">
+      <c r="F169" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H169" s="14" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A174" t="s">
-        <v>197</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A175" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A176" t="s">
+        <v>199</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A177" t="s">
         <v>201</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="B177" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C177" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E176" s="1" t="s">
+      <c r="D177" s="4"/>
+      <c r="E177" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F176" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H176" s="2" t="s">
+      <c r="F177" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G177" s="4"/>
+      <c r="H177" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C177" t="s">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C178" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E177" s="1" t="s">
+      <c r="D178" s="4"/>
+      <c r="E178" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F177" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H177" s="2" t="s">
+      <c r="F178" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G178" s="4"/>
+      <c r="H178" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C178" t="s">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C179" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E178" s="4" t="s">
+      <c r="D179" s="4"/>
+      <c r="E179" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="F178" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H178" s="2" t="s">
+      <c r="F179" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G179" s="4"/>
+      <c r="H179" s="5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C179" t="s">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C180" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E179" s="4" t="s">
+      <c r="D180" s="4"/>
+      <c r="E180" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F179" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H179" s="2" t="s">
+      <c r="F180" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G180" s="4"/>
+      <c r="H180" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C180" t="s">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C181" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E180" s="8" t="s">
+      <c r="D181" s="4"/>
+      <c r="E181" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F180" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H180" s="2" t="s">
+      <c r="F181" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G181" s="4"/>
+      <c r="H181" s="5" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C181" t="s">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C182" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E181" s="1" t="s">
+      <c r="D182" s="4"/>
+      <c r="E182" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F181" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H181" s="2" t="s">
+      <c r="F182" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G182" s="4"/>
+      <c r="H182" s="5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A182" t="s">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A183" t="s">
         <v>304</v>
       </c>
-      <c r="B182" s="1" t="s">
+      <c r="B183" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C183" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="D182" s="1" t="s">
+      <c r="D183" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E182" s="1" t="s">
+      <c r="E183" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F182" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G182" s="1" t="s">
+      <c r="F183" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G183" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="H182" s="14" t="s">
+      <c r="H183" s="15" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C183" t="s">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C184" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="E183" s="1" t="s">
+      <c r="D184" s="4"/>
+      <c r="E184" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F183" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H183" t="s">
+      <c r="F184" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G184" s="4"/>
+      <c r="H184" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C184" t="s">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C185" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="E184" s="1" t="s">
+      <c r="D185" s="4"/>
+      <c r="E185" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F184" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H184" t="s">
+      <c r="F185" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G185" s="4"/>
+      <c r="H185" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C185" t="s">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C186" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="E185" s="1" t="s">
+      <c r="D186" s="4"/>
+      <c r="E186" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F185" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G185" s="1">
+      <c r="F186" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G186" s="4">
         <v>1</v>
       </c>
-      <c r="H185" t="s">
+      <c r="H186" s="3" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C186" t="s">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C187" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E186" s="1" t="s">
+      <c r="D187" s="4"/>
+      <c r="E187" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F186" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G186" s="1" t="s">
+      <c r="F187" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G187" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H186" t="s">
+      <c r="H187" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C187" t="s">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C188" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="E187" s="1" t="s">
+      <c r="D188" s="4"/>
+      <c r="E188" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F187" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H187" s="14" t="s">
+      <c r="F188" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G188" s="4"/>
+      <c r="H188" s="15" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C188" t="s">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C189" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="E188" s="1" t="s">
+      <c r="D189" s="4"/>
+      <c r="E189" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F188" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H188" s="14" t="s">
+      <c r="F189" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G189" s="4"/>
+      <c r="H189" s="15" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C189" t="s">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C190" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E189" s="1" t="s">
+      <c r="D190" s="4"/>
+      <c r="E190" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F189" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H189" s="14" t="s">
+      <c r="F190" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G190" s="4"/>
+      <c r="H190" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C190" t="s">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C191" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="E190" s="1" t="s">
+      <c r="D191" s="4"/>
+      <c r="E191" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F190" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H190" s="14" t="s">
+      <c r="F191" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G191" s="4"/>
+      <c r="H191" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A191" t="s">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A192" t="s">
         <v>317</v>
       </c>
-      <c r="B191" s="1" t="s">
+      <c r="B192" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C191" s="7" t="s">
+      <c r="C192" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="D191" s="8" t="s">
+      <c r="D192" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E191" s="8" t="s">
+      <c r="E192" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F191" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G191" s="8" t="s">
+      <c r="F192" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G192" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="H191" s="7" t="s">
+      <c r="H192" s="3" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C192" s="7" t="s">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C193" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D192" s="8" t="s">
+      <c r="D193" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E192" s="8" t="s">
+      <c r="E193" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F192" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G192" s="8"/>
-      <c r="H192" s="7" t="s">
+      <c r="F193" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G193" s="4"/>
+      <c r="H193" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="193" spans="3:8" x14ac:dyDescent="0.4">
-      <c r="C193" s="7" t="s">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C194" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D193" s="8"/>
-      <c r="E193" s="8" t="s">
+      <c r="D194" s="4"/>
+      <c r="E194" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="F193" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G193" s="8"/>
-      <c r="H193" s="7" t="s">
+      <c r="F194" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G194" s="4"/>
+      <c r="H194" s="3" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="194" spans="3:8" x14ac:dyDescent="0.4">
-      <c r="C194" t="s">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C195" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="E194" s="1" t="s">
+      <c r="D195" s="4"/>
+      <c r="E195" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F194" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H194" s="14" t="s">
+      <c r="F195" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G195" s="4"/>
+      <c r="H195" s="15" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="195" spans="3:8" x14ac:dyDescent="0.4">
-      <c r="C195" t="s">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C196" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="E195" s="1" t="s">
+      <c r="D196" s="4"/>
+      <c r="E196" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F195" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H195" s="14" t="s">
+      <c r="F196" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G196" s="4"/>
+      <c r="H196" s="15" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A197" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="C197" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D197" s="8"/>
+      <c r="E197" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F197" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G197" s="8"/>
+      <c r="H197" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A198" s="7"/>
+      <c r="B198" s="8"/>
+      <c r="C198" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="D198" s="8"/>
+      <c r="E198" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F198" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G198" s="8"/>
+      <c r="H198" s="9" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021-05-21 결제테이블 추가 commit
</commit_message>
<xml_diff>
--- a/src/main/document/협회TABLE.xlsx
+++ b/src/main/document/협회TABLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF9236A-5AA8-4A7F-96A7-DC8254672EC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742C7A2E-A068-47FF-8A26-25AC24E901BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="346">
   <si>
     <t>테이블명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -240,14 +240,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>결제내역</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결제정보 전달 받은 후 기재</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>결제내역이력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -846,10 +838,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>결제내역시퀀스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>모집인변경이력시퀀스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1297,6 +1285,80 @@
   </si>
   <si>
     <t>법인사용인여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tb_lc_pay_seq</t>
+  </si>
+  <si>
+    <t>ORDER_NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAY_TYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEQ_NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APPROVAL_NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELL_MM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제정보</t>
+  </si>
+  <si>
+    <t>결제시퀀스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지불수단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거래일련번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>승인번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카드/은행ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카드/은행명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>할부개월</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금액</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1791,10 +1853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K198"/>
+  <dimension ref="A2:K208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D183" sqref="D183"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1824,7 +1886,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>3</v>
@@ -1838,39 +1900,39 @@
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
@@ -1878,10 +1940,10 @@
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>10</v>
@@ -1889,30 +1951,30 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
@@ -1920,10 +1982,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>11</v>
@@ -1931,18 +1993,18 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C9" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
@@ -1950,13 +2012,13 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
@@ -1965,10 +2027,10 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="5" t="s">
@@ -1981,14 +2043,14 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
@@ -1997,10 +2059,10 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="5" t="s">
@@ -2009,102 +2071,102 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C14" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C15" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C16" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C17" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="9" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C18" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="9" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C19" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
@@ -2113,139 +2175,139 @@
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="7" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B21" s="4"/>
       <c r="C21" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B22" s="4"/>
       <c r="C22" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G22" s="4">
         <v>0</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B23" s="4"/>
       <c r="C23" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B24" s="4"/>
       <c r="C24" s="7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="9" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B25" s="4"/>
       <c r="C25" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B26" s="4"/>
       <c r="C26" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B27" s="4"/>
       <c r="C27" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
@@ -2253,53 +2315,53 @@
         <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C29" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C30" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5" t="s">
@@ -2310,14 +2372,14 @@
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5" t="s">
@@ -2332,142 +2394,142 @@
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.4">
@@ -2475,96 +2537,96 @@
         <v>19</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C43" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C44" s="7" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.4">
@@ -2573,49 +2635,49 @@
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C46" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C47" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>20</v>
@@ -2623,20 +2685,20 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C48" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H48" s="13" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
@@ -2644,14 +2706,14 @@
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C49" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="5" t="s">
@@ -2663,14 +2725,14 @@
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C50" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="5" t="s">
@@ -2682,18 +2744,18 @@
     </row>
     <row r="51" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C51" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
@@ -2701,14 +2763,14 @@
     </row>
     <row r="52" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C52" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="5" t="s">
@@ -2720,18 +2782,18 @@
     </row>
     <row r="53" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C53" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
@@ -2739,14 +2801,14 @@
     </row>
     <row r="54" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C54" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="5" t="s">
@@ -2762,16 +2824,16 @@
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
@@ -2779,18 +2841,18 @@
     </row>
     <row r="56" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C56" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
@@ -2798,14 +2860,14 @@
     </row>
     <row r="57" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C57" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>37</v>
@@ -2813,14 +2875,14 @@
     </row>
     <row r="58" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C58" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>39</v>
@@ -2828,14 +2890,14 @@
     </row>
     <row r="59" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C59" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>40</v>
@@ -2843,14 +2905,14 @@
     </row>
     <row r="60" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C60" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>41</v>
@@ -2858,14 +2920,14 @@
     </row>
     <row r="61" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C61" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>44</v>
@@ -2873,14 +2935,14 @@
     </row>
     <row r="62" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C62" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>24</v>
@@ -2888,30 +2950,30 @@
     </row>
     <row r="63" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C63" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="64" spans="3:11" x14ac:dyDescent="0.4">
       <c r="C64" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>14</v>
@@ -2919,14 +2981,14 @@
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C65" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>15</v>
@@ -2938,25 +3000,25 @@
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C67" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="5" t="s">
@@ -2970,10 +3032,10 @@
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G68" s="4"/>
       <c r="H68" s="5" t="s">
@@ -2983,14 +3045,14 @@
     </row>
     <row r="69" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C69" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G69" s="4"/>
       <c r="H69" s="5" t="s">
@@ -3000,14 +3062,14 @@
     </row>
     <row r="70" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C70" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G70" s="4"/>
       <c r="H70" s="5" t="s">
@@ -3017,33 +3079,33 @@
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C71" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I71" s="3"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C72" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G72" s="4"/>
       <c r="H72" s="5" t="s">
@@ -3053,14 +3115,14 @@
     </row>
     <row r="73" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C73" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G73" s="4"/>
       <c r="H73" s="5" t="s">
@@ -3070,14 +3132,14 @@
     </row>
     <row r="74" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C74" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="5" t="s">
@@ -3091,10 +3153,10 @@
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G75" s="4"/>
       <c r="H75" s="5" t="s">
@@ -3104,103 +3166,103 @@
     </row>
     <row r="76" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C76" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G76" s="4"/>
       <c r="H76" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="I76" s="3"/>
     </row>
     <row r="77" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C77" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G77" s="4"/>
       <c r="H77" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="I77" s="3"/>
     </row>
     <row r="78" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C78" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G78" s="4"/>
       <c r="H78" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I78" s="3"/>
     </row>
     <row r="79" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C79" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G79" s="4"/>
       <c r="H79" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I79" s="3"/>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C80" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G80" s="4"/>
       <c r="H80" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I80" s="3"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C81" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G81" s="4"/>
       <c r="H81" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I81" s="3"/>
     </row>
@@ -3208,18 +3270,18 @@
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G82" s="4"/>
       <c r="H82" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I82" s="3"/>
     </row>
@@ -3227,18 +3289,18 @@
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G83" s="4"/>
       <c r="H83" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.4">
@@ -3246,39 +3308,39 @@
         <v>48</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C85" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G85" s="4"/>
       <c r="H85" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.4">
@@ -3287,16 +3349,16 @@
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.4">
@@ -3305,42 +3367,42 @@
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G87" s="4"/>
       <c r="H87" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C88" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C89" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="5" t="s">
@@ -3349,14 +3411,14 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C90" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="5" t="s">
@@ -3365,14 +3427,14 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C91" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G91" s="4"/>
       <c r="H91" s="5" t="s">
@@ -3381,14 +3443,14 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C92" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="5" t="s">
@@ -3397,54 +3459,54 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C93" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C94" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C95" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G95" s="4"/>
       <c r="H95" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.4">
@@ -3452,39 +3514,39 @@
         <v>50</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C97" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.4">
@@ -3493,26 +3555,26 @@
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C99" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="5" t="s">
@@ -3521,14 +3583,14 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C100" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="5" t="s">
@@ -3537,17 +3599,17 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C101" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>37</v>
@@ -3555,14 +3617,14 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C102" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G102" s="4"/>
       <c r="H102" s="5" t="s">
@@ -3571,14 +3633,14 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C103" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="5" t="s">
@@ -3587,18 +3649,18 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C104" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.4">
@@ -3606,51 +3668,51 @@
         <v>51</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H105" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C106" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G106" s="4"/>
       <c r="H106" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C107" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G107" s="4"/>
       <c r="H107" s="5" t="s">
@@ -3659,14 +3721,14 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C108" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G108" s="4"/>
       <c r="H108" s="5" t="s">
@@ -3675,18 +3737,18 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C109" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G109" s="4"/>
       <c r="H109" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.4">
@@ -3694,51 +3756,51 @@
         <v>52</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C111" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G111" s="4"/>
       <c r="H111" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C112" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G112" s="4"/>
       <c r="H112" s="5" t="s">
@@ -3747,66 +3809,66 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C113" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G113" s="4"/>
       <c r="H113" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C114" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G114" s="4"/>
       <c r="H114" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C115" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G115" s="4"/>
       <c r="H115" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C116" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G116" s="4"/>
       <c r="H116" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.4">
@@ -3814,30 +3876,30 @@
         <v>53</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D117" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H117" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C118" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -3846,1200 +3908,1393 @@
       <c r="H118" s="5"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A119" t="s">
+      <c r="A119" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E119" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F119" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G119" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="H119" s="9" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A120" s="7"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F120" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G120" s="8"/>
+      <c r="H120" s="9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A121" s="7"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D121" s="8"/>
+      <c r="E121" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F121" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G121" s="8"/>
+      <c r="H121" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A122" s="7"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F122" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G122" s="8"/>
+      <c r="H122" s="9" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A123" s="7"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="D123" s="8"/>
+      <c r="E123" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F123" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G123" s="8"/>
+      <c r="H123" s="9" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A124" s="7"/>
+      <c r="B124" s="8"/>
+      <c r="C124" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F124" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G124" s="8"/>
+      <c r="H124" s="9" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A125" s="7"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="D125" s="8"/>
+      <c r="E125" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F125" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G125" s="8"/>
+      <c r="H125" s="9" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A126" s="7"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="D126" s="8"/>
+      <c r="E126" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F126" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G126" s="8"/>
+      <c r="H126" s="9" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A127" s="7"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="D127" s="8"/>
+      <c r="E127" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F127" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G127" s="8"/>
+      <c r="H127" s="9" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A128" s="7"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F128" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G128" s="8"/>
+      <c r="H128" s="9" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A129" s="7"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D129" s="8"/>
+      <c r="E129" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F129" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G129" s="8"/>
+      <c r="H129" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A130" s="7"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F130" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G130" s="8"/>
+      <c r="H130" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A131" t="s">
         <v>54</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D119" s="4" t="s">
+      <c r="B131" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C131" t="s">
+        <v>206</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E119" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F119" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G119" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="H119" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C120" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A121" t="s">
-        <v>56</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C121" t="s">
-        <v>208</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H121" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C122" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A123" t="s">
-        <v>59</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C123" t="s">
-        <v>192</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G123" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H123" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C124" t="s">
-        <v>235</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G124" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="H124" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C125" t="s">
-        <v>103</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H125" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C126" t="s">
-        <v>87</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H126" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C127" t="s">
-        <v>106</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H127" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C128" t="s">
-        <v>91</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H128" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C129" t="s">
-        <v>94</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H129" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C130" t="s">
-        <v>194</v>
-      </c>
-      <c r="E130" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H130" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C131" t="s">
-        <v>139</v>
-      </c>
       <c r="E131" s="1" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>142</v>
+        <v>207</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C132" t="s">
-        <v>99</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H132" s="2" t="s">
-        <v>123</v>
+        <v>55</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C133" t="s">
-        <v>107</v>
+        <v>190</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="H133" s="2" t="s">
-        <v>115</v>
+        <v>191</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C134" t="s">
-        <v>108</v>
+        <v>232</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>116</v>
+        <v>233</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C135" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C136" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C137" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C138" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C139" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C140" t="s">
-        <v>114</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>92</v>
+        <v>192</v>
+      </c>
+      <c r="E140" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C141" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G141" s="1" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C142" t="s">
-        <v>194</v>
+        <v>97</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A143" t="s">
+        <v>58</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="C143" t="s">
-        <v>170</v>
+        <v>105</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>171</v>
+        <v>113</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C144" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C145" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H145" s="2" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A146" t="s">
-        <v>61</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="C146" t="s">
-        <v>107</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C147" t="s">
-        <v>124</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C148" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C149" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C150" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C151" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C152" t="s">
-        <v>112</v>
+        <v>192</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C153" t="s">
-        <v>113</v>
+        <v>168</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>121</v>
+        <v>169</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C154" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C155" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G155" s="1" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="H155" s="2" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A156" t="s">
+        <v>59</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="C156" t="s">
-        <v>194</v>
+        <v>105</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C157" t="s">
-        <v>170</v>
+        <v>122</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C158" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H158" s="2" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C159" t="s">
+        <v>125</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H159" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C160" t="s">
+        <v>108</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H160" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C161" t="s">
+        <v>109</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H161" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C162" t="s">
+        <v>110</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H162" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C163" t="s">
+        <v>111</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H163" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C164" t="s">
+        <v>112</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H164" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C165" t="s">
+        <v>96</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H165" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C166" t="s">
+        <v>192</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H166" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C167" t="s">
+        <v>168</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H167" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C168" t="s">
+        <v>137</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H168" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E159" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F159" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H159" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A160" t="s">
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C169" t="s">
+        <v>138</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H169" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A170" t="s">
+        <v>267</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C170" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="H170" s="14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C171" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H171" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="B160" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="C160" s="14" t="s">
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C172" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H172" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D160" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F160" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="H160" s="14" t="s">
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C173" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G173" s="1">
+        <v>0</v>
+      </c>
+      <c r="H173" s="14" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C161" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F161" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H161" s="14" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C162" s="14" t="s">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C174" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H174" s="14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C175" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="E162" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F162" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H162" s="14" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C163" s="14" t="s">
+      <c r="E175" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H175" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="E163" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G163" s="1">
-        <v>0</v>
-      </c>
-      <c r="H163" s="14" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C164" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F164" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H164" s="14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C165" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F165" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G165" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H165" s="14" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C166" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F166" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H166" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C167" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F167" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H167" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C168" s="14" t="s">
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C176" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H176" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C177" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H177" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C178" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H178" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C179" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H179" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E168" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H168" s="14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C169" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F169" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H169" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A175" t="s">
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A185" t="s">
+        <v>195</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A186" t="s">
         <v>197</v>
       </c>
-      <c r="B175" s="1" t="s">
+      <c r="B186" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A176" t="s">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A187" t="s">
         <v>199</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="B187" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A177" t="s">
-        <v>201</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D177" s="4"/>
-      <c r="E177" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F177" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G177" s="4"/>
-      <c r="H177" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C178" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D178" s="4"/>
-      <c r="E178" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F178" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G178" s="4"/>
-      <c r="H178" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C179" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D179" s="4"/>
-      <c r="E179" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="F179" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G179" s="4"/>
-      <c r="H179" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C180" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D180" s="4"/>
-      <c r="E180" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F180" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G180" s="4"/>
-      <c r="H180" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C181" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D181" s="4"/>
-      <c r="E181" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F181" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G181" s="4"/>
-      <c r="H181" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C182" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D182" s="4"/>
-      <c r="E182" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F182" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G182" s="4"/>
-      <c r="H182" s="5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A183" t="s">
-        <v>304</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="D183" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E183" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F183" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G183" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="H183" s="15" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C184" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="D184" s="4"/>
-      <c r="E184" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F184" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G184" s="4"/>
-      <c r="H184" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C185" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="D185" s="4"/>
-      <c r="E185" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="F185" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G185" s="4"/>
-      <c r="H185" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C186" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D186" s="4"/>
-      <c r="E186" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F186" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G186" s="4">
-        <v>1</v>
-      </c>
-      <c r="H186" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C187" s="3" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="D187" s="4"/>
       <c r="E187" s="4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F187" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G187" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="H187" s="3" t="s">
-        <v>123</v>
+        <v>65</v>
+      </c>
+      <c r="G187" s="4"/>
+      <c r="H187" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C188" s="3" t="s">
-        <v>313</v>
+        <v>154</v>
       </c>
       <c r="D188" s="4"/>
       <c r="E188" s="4" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="F188" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G188" s="4"/>
-      <c r="H188" s="15" t="s">
-        <v>96</v>
+      <c r="H188" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C189" s="3" t="s">
-        <v>314</v>
+        <v>149</v>
       </c>
       <c r="D189" s="4"/>
       <c r="E189" s="4" t="s">
-        <v>72</v>
+        <v>246</v>
       </c>
       <c r="F189" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G189" s="4"/>
-      <c r="H189" s="15" t="s">
-        <v>171</v>
+      <c r="H189" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C190" s="3" t="s">
-        <v>315</v>
+        <v>150</v>
       </c>
       <c r="D190" s="4"/>
       <c r="E190" s="4" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="F190" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G190" s="4"/>
-      <c r="H190" s="15" t="s">
-        <v>142</v>
+      <c r="H190" s="5" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C191" s="3" t="s">
-        <v>316</v>
+        <v>156</v>
       </c>
       <c r="D191" s="4"/>
       <c r="E191" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F191" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G191" s="4"/>
-      <c r="H191" s="15" t="s">
-        <v>141</v>
+      <c r="H191" s="5" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A192" t="s">
-        <v>317</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>318</v>
-      </c>
       <c r="C192" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="D192" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="D192" s="4"/>
       <c r="E192" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F192" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G192" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="H192" s="3" t="s">
-        <v>321</v>
+        <v>65</v>
+      </c>
+      <c r="G192" s="4"/>
+      <c r="H192" s="5" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A193" t="s">
+        <v>301</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>302</v>
+      </c>
       <c r="C193" s="3" t="s">
-        <v>176</v>
+        <v>303</v>
       </c>
       <c r="D193" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E193" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F193" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G193" s="4"/>
-      <c r="H193" s="3" t="s">
-        <v>177</v>
+        <v>65</v>
+      </c>
+      <c r="G193" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H193" s="15" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C194" s="3" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="D194" s="4"/>
       <c r="E194" s="4" t="s">
-        <v>302</v>
+        <v>68</v>
       </c>
       <c r="F194" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G194" s="4"/>
       <c r="H194" s="3" t="s">
-        <v>323</v>
+        <v>24</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C195" s="3" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D195" s="4"/>
       <c r="E195" s="4" t="s">
-        <v>104</v>
+        <v>176</v>
       </c>
       <c r="F195" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G195" s="4"/>
-      <c r="H195" s="15" t="s">
-        <v>96</v>
+      <c r="H195" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C196" s="3" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D196" s="4"/>
       <c r="E196" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F196" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G196" s="4"/>
-      <c r="H196" s="15" t="s">
-        <v>171</v>
+        <v>65</v>
+      </c>
+      <c r="G196" s="4">
+        <v>1</v>
+      </c>
+      <c r="H196" s="3" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A197" s="7" t="s">
+      <c r="C197" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D197" s="4"/>
+      <c r="E197" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F197" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G197" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H197" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C198" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D198" s="4"/>
+      <c r="E198" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F198" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G198" s="4"/>
+      <c r="H198" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C199" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D199" s="4"/>
+      <c r="E199" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F199" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G199" s="4"/>
+      <c r="H199" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C200" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="D200" s="4"/>
+      <c r="E200" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F200" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G200" s="4"/>
+      <c r="H200" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C201" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D201" s="4"/>
+      <c r="E201" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F201" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G201" s="4"/>
+      <c r="H201" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A202" t="s">
+        <v>314</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E202" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F202" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G202" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="H202" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C203" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E203" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F203" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G203" s="4"/>
+      <c r="H203" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C204" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D204" s="4"/>
+      <c r="E204" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F204" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G204" s="4"/>
+      <c r="H204" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C205" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D205" s="4"/>
+      <c r="E205" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F205" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G205" s="4"/>
+      <c r="H205" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C206" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D206" s="4"/>
+      <c r="E206" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F206" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G206" s="4"/>
+      <c r="H206" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A207" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="B207" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C207" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D207" s="8"/>
+      <c r="E207" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F207" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G207" s="8"/>
+      <c r="H207" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A208" s="7"/>
+      <c r="B208" s="8"/>
+      <c r="C208" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="D208" s="8"/>
+      <c r="E208" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F208" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G208" s="8"/>
+      <c r="H208" s="9" t="s">
         <v>324</v>
-      </c>
-      <c r="B197" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="C197" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D197" s="8"/>
-      <c r="E197" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F197" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G197" s="8"/>
-      <c r="H197" s="9" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A198" s="7"/>
-      <c r="B198" s="8"/>
-      <c r="C198" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="D198" s="8"/>
-      <c r="E198" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F198" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G198" s="8"/>
-      <c r="H198" s="9" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -5077,16 +5332,16 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>117</v>
-      </c>
       <c r="E2" s="11" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>

</xml_diff>

<commit_message>
2021-05-31 table_ddl 추가 및 테이블정의서 추가 commit
</commit_message>
<xml_diff>
--- a/src/main/document/협회TABLE.xlsx
+++ b/src/main/document/협회TABLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF6770B-4870-45D4-95CE-419C854B6CDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E3E39A-C5CA-48E8-AA02-82D0355C8A41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="351">
   <si>
     <t>테이블명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1375,6 +1375,10 @@
   </si>
   <si>
     <t>승인남은일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>암호화</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1871,8 +1875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1885,9 +1889,10 @@
     <col min="6" max="6" width="13.69921875" style="1" customWidth="1"/>
     <col min="7" max="7" width="33.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="39" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
         <v>0</v>
@@ -1910,8 +1915,11 @@
       <c r="H2" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I2" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1937,7 +1945,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C4" t="s">
         <v>131</v>
       </c>
@@ -1951,7 +1959,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C5" t="s">
         <v>5</v>
       </c>
@@ -1965,7 +1973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
         <v>132</v>
       </c>
@@ -1979,7 +1987,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
         <v>136</v>
       </c>
@@ -1993,21 +2001,23 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C8" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="F8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C9" s="3" t="s">
         <v>251</v>
       </c>
@@ -2023,21 +2033,23 @@
         <v>252</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C10" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="F10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
@@ -2053,7 +2065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
@@ -2069,7 +2081,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C13" s="3" t="s">
         <v>28</v>
       </c>
@@ -2085,7 +2097,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C14" s="3" t="s">
         <v>75</v>
       </c>
@@ -2101,7 +2113,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C15" s="3" t="s">
         <v>254</v>
       </c>
@@ -2119,7 +2131,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C16" s="3" t="s">
         <v>257</v>
       </c>
@@ -2135,39 +2147,39 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C17" s="7" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C17" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9" t="s">
+      <c r="F17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="5" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C18" s="7" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C18" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9" t="s">
+      <c r="F18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="5" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C19" s="3" t="s">
         <v>262</v>
       </c>
@@ -2185,23 +2197,23 @@
         <v>288</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C20" s="7" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C20" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7" t="s">
+      <c r="F20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="3" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B21" s="4"/>
       <c r="C21" s="3" t="s">
         <v>190</v>
@@ -2218,7 +2230,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B22" s="4"/>
       <c r="C22" s="3" t="s">
         <v>60</v>
@@ -2237,7 +2249,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B23" s="4"/>
       <c r="C23" s="3" t="s">
         <v>82</v>
@@ -2256,24 +2268,24 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B24" s="4"/>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8" t="s">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9" t="s">
+      <c r="F24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="5" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B25" s="4"/>
       <c r="C25" s="3" t="s">
         <v>78</v>
@@ -2292,7 +2304,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B26" s="4"/>
       <c r="C26" s="3" t="s">
         <v>138</v>
@@ -2309,7 +2321,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B27" s="4"/>
       <c r="C27" s="3" t="s">
         <v>137</v>
@@ -2326,7 +2338,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -2352,7 +2364,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C29" s="3" t="s">
         <v>142</v>
       </c>
@@ -2368,13 +2380,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C30" s="3" t="s">
         <v>143</v>
       </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="4" t="s">
-        <v>176</v>
+      <c r="E30" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>74</v>
@@ -2383,8 +2395,11 @@
       <c r="H30" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I30" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3" t="s">
@@ -2402,7 +2417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3" t="s">
@@ -2628,20 +2643,20 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8" t="s">
+      <c r="D44" s="4"/>
+      <c r="E44" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F44" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G44" s="8" t="s">
+      <c r="F44" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G44" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H44" s="9" t="s">
+      <c r="H44" s="5" t="s">
         <v>326</v>
       </c>
     </row>
@@ -2782,8 +2797,8 @@
         <v>154</v>
       </c>
       <c r="D52" s="4"/>
-      <c r="E52" s="4" t="s">
-        <v>62</v>
+      <c r="E52" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>74</v>
@@ -2792,7 +2807,9 @@
       <c r="H52" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I52" s="3"/>
+      <c r="I52" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
     </row>
@@ -2985,14 +3002,17 @@
         <v>143</v>
       </c>
       <c r="D64" s="4"/>
-      <c r="E64" s="4" t="s">
-        <v>176</v>
+      <c r="E64" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.4">
@@ -3113,35 +3133,35 @@
       <c r="I71" s="3"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8" t="s">
+      <c r="D72" s="4"/>
+      <c r="E72" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F72" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G72" s="8"/>
-      <c r="H72" s="9" t="s">
+      <c r="F72" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G72" s="4"/>
+      <c r="H72" s="5" t="s">
         <v>347</v>
       </c>
       <c r="I72" s="3"/>
     </row>
     <row r="73" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="C73" s="7" t="s">
+      <c r="C73" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8" t="s">
+      <c r="D73" s="4"/>
+      <c r="E73" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F73" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G73" s="8"/>
-      <c r="H73" s="9" t="s">
+      <c r="F73" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G73" s="4"/>
+      <c r="H73" s="5" t="s">
         <v>349</v>
       </c>
       <c r="I73" s="3"/>
@@ -3448,8 +3468,8 @@
         <v>154</v>
       </c>
       <c r="D91" s="4"/>
-      <c r="E91" s="4" t="s">
-        <v>62</v>
+      <c r="E91" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="F91" s="4" t="s">
         <v>74</v>
@@ -3458,6 +3478,9 @@
       <c r="H91" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="I91" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C92" s="3" t="s">
@@ -3543,7 +3566,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C97" s="3" t="s">
         <v>189</v>
       </c>
@@ -3559,7 +3582,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>50</v>
       </c>
@@ -3583,7 +3606,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C99" s="3" t="s">
         <v>174</v>
       </c>
@@ -3599,7 +3622,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C100" s="3" t="s">
         <v>49</v>
       </c>
@@ -3615,7 +3638,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C101" s="3" t="s">
         <v>227</v>
       </c>
@@ -3631,13 +3654,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C102" s="3" t="s">
         <v>154</v>
       </c>
       <c r="D102" s="4"/>
-      <c r="E102" s="4" t="s">
-        <v>62</v>
+      <c r="E102" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="F102" s="4" t="s">
         <v>74</v>
@@ -3646,8 +3669,11 @@
       <c r="H102" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I102" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C103" s="3" t="s">
         <v>177</v>
       </c>
@@ -3665,7 +3691,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C104" s="3" t="s">
         <v>214</v>
       </c>
@@ -3681,7 +3707,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C105" s="3" t="s">
         <v>216</v>
       </c>
@@ -3697,7 +3723,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C106" s="3" t="s">
         <v>189</v>
       </c>
@@ -3713,7 +3739,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
         <v>51</v>
       </c>
@@ -3737,7 +3763,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C108" s="3" t="s">
         <v>174</v>
       </c>
@@ -3753,7 +3779,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C109" s="3" t="s">
         <v>228</v>
       </c>
@@ -3769,13 +3795,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C110" s="3" t="s">
         <v>154</v>
       </c>
       <c r="D110" s="4"/>
-      <c r="E110" s="4" t="s">
-        <v>62</v>
+      <c r="E110" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="F110" s="4" t="s">
         <v>74</v>
@@ -3784,8 +3810,11 @@
       <c r="H110" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I110" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C111" s="3" t="s">
         <v>189</v>
       </c>
@@ -3801,7 +3830,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
         <v>52</v>
       </c>

</xml_diff>